<commit_message>
update mapping : generic PMT update
</commit_message>
<xml_diff>
--- a/mapping/mapping_TB2021July_v1.xlsx
+++ b/mapping/mapping_TB2021July_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khwang/scratch/TB2023July/preparation/dev_230622/TB2023/mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAD8497-DDB7-BC4D-99AB-27EF9D5D48D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051377B8-894E-9944-A00A-078FBF1ECD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13100" yWindow="500" windowWidth="55700" windowHeight="28300" activeTab="1" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
+    <workbookView xWindow="23080" yWindow="500" windowWidth="45720" windowHeight="28300" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
   </bookViews>
   <sheets>
     <sheet name="dynamic" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="167">
   <si>
     <t>MID</t>
   </si>
@@ -1005,11 +1005,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FA2B49-E75F-9B4E-BCDE-F5B7F2A15CFB}">
-  <dimension ref="A1:W289"/>
+  <dimension ref="A1:Y289"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R235" sqref="R235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5937,7 +5937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>6</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>8</v>
       </c>
@@ -5995,8 +5995,12 @@
         <v>0</v>
       </c>
       <c r="H194" s="10"/>
-      <c r="I194" s="10"/>
-      <c r="J194" s="10"/>
+      <c r="I194" s="10">
+        <v>0</v>
+      </c>
+      <c r="J194" s="10">
+        <v>0</v>
+      </c>
       <c r="M194">
         <f>IF(L194 = $O$193, 0,  VLOOKUP(L194,$R$190:$S$194, 2, FALSE))</f>
         <v>0</v>
@@ -6015,8 +6019,10 @@
       <c r="S194">
         <v>14</v>
       </c>
-    </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X194" s="10"/>
+      <c r="Y194" s="10"/>
+    </row>
+    <row r="195" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>8</v>
       </c>
@@ -6069,8 +6075,10 @@
       <c r="S195">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X195" s="10"/>
+      <c r="Y195" s="10"/>
+    </row>
+    <row r="196" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>8</v>
       </c>
@@ -6096,8 +6104,12 @@
         <v>0</v>
       </c>
       <c r="H196" s="10"/>
-      <c r="I196" s="10"/>
-      <c r="J196" s="10"/>
+      <c r="I196" s="10">
+        <v>0</v>
+      </c>
+      <c r="J196" s="10">
+        <v>0</v>
+      </c>
       <c r="M196">
         <f t="shared" ref="M196:M257" si="5">IF(L196 = $O$193, 0,  VLOOKUP(L196,$R$190:$S$194, 2, FALSE))</f>
         <v>0</v>
@@ -6110,8 +6122,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X196" s="10"/>
+      <c r="Y196" s="10"/>
+    </row>
+    <row r="197" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>8</v>
       </c>
@@ -6124,7 +6138,7 @@
       </c>
       <c r="D197" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E197" s="10">
         <f t="shared" si="3"/>
@@ -6138,10 +6152,10 @@
       </c>
       <c r="H197" s="10"/>
       <c r="I197" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J197" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K197" t="s">
         <v>42</v>
@@ -6155,14 +6169,16 @@
       </c>
       <c r="N197">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O197">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X197" s="10"/>
+      <c r="Y197" s="10"/>
+    </row>
+    <row r="198" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>8</v>
       </c>
@@ -6188,8 +6204,12 @@
         <v>0</v>
       </c>
       <c r="H198" s="10"/>
-      <c r="I198" s="10"/>
-      <c r="J198" s="10"/>
+      <c r="I198" s="10">
+        <v>0</v>
+      </c>
+      <c r="J198" s="10">
+        <v>0</v>
+      </c>
       <c r="M198">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6211,8 +6231,10 @@
       <c r="W198" s="19" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X198" s="10"/>
+      <c r="Y198" s="10"/>
+    </row>
+    <row r="199" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>8</v>
       </c>
@@ -6280,8 +6302,10 @@
       <c r="W199" s="19" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X199" s="10"/>
+      <c r="Y199" s="10"/>
+    </row>
+    <row r="200" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>8</v>
       </c>
@@ -6307,8 +6331,12 @@
         <v>0</v>
       </c>
       <c r="H200" s="10"/>
-      <c r="I200" s="10"/>
-      <c r="J200" s="10"/>
+      <c r="I200" s="10">
+        <v>0</v>
+      </c>
+      <c r="J200" s="10">
+        <v>0</v>
+      </c>
       <c r="M200">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6336,8 +6364,10 @@
       <c r="W200" s="19" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X200" s="10"/>
+      <c r="Y200" s="10"/>
+    </row>
+    <row r="201" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>8</v>
       </c>
@@ -6350,7 +6380,7 @@
       </c>
       <c r="D201" s="10">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E201" s="10">
         <f t="shared" si="3"/>
@@ -6364,10 +6394,10 @@
       </c>
       <c r="H201" s="10"/>
       <c r="I201" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J201" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K201" t="s">
         <v>42</v>
@@ -6381,7 +6411,7 @@
       </c>
       <c r="N201">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O201">
         <f t="shared" si="4"/>
@@ -6402,8 +6432,10 @@
       <c r="W201" s="19" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X201" s="10"/>
+      <c r="Y201" s="10"/>
+    </row>
+    <row r="202" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>8</v>
       </c>
@@ -6429,8 +6461,12 @@
         <v>0</v>
       </c>
       <c r="H202" s="10"/>
-      <c r="I202" s="10"/>
-      <c r="J202" s="10"/>
+      <c r="I202" s="10">
+        <v>0</v>
+      </c>
+      <c r="J202" s="10">
+        <v>0</v>
+      </c>
       <c r="M202">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6458,8 +6494,10 @@
       <c r="W202" s="19" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X202" s="10"/>
+      <c r="Y202" s="10"/>
+    </row>
+    <row r="203" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>8</v>
       </c>
@@ -6472,7 +6510,7 @@
       </c>
       <c r="D203" s="10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E203" s="10">
         <f t="shared" si="3"/>
@@ -6486,10 +6524,10 @@
       </c>
       <c r="H203" s="10"/>
       <c r="I203" s="10" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J203" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K203" t="s">
         <v>42</v>
@@ -6503,7 +6541,7 @@
       </c>
       <c r="N203">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O203">
         <f t="shared" si="4"/>
@@ -6511,8 +6549,10 @@
       </c>
       <c r="V203" s="19"/>
       <c r="W203" s="19"/>
-    </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X203" s="10"/>
+      <c r="Y203" s="10"/>
+    </row>
+    <row r="204" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>8</v>
       </c>
@@ -6538,8 +6578,12 @@
         <v>0</v>
       </c>
       <c r="H204" s="10"/>
-      <c r="I204" s="10"/>
-      <c r="J204" s="10"/>
+      <c r="I204" s="10">
+        <v>0</v>
+      </c>
+      <c r="J204" s="10">
+        <v>0</v>
+      </c>
       <c r="M204">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6570,8 +6614,10 @@
       <c r="W204" s="19" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X204" s="10"/>
+      <c r="Y204" s="10"/>
+    </row>
+    <row r="205" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>8</v>
       </c>
@@ -6584,7 +6630,7 @@
       </c>
       <c r="D205" s="10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E205" s="10">
         <f t="shared" si="3"/>
@@ -6598,10 +6644,10 @@
       </c>
       <c r="H205" s="10"/>
       <c r="I205" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J205" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K205" t="s">
         <v>42</v>
@@ -6615,7 +6661,7 @@
       </c>
       <c r="N205">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O205">
         <f t="shared" si="4"/>
@@ -6636,8 +6682,10 @@
       <c r="W205" s="19" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X205" s="10"/>
+      <c r="Y205" s="10"/>
+    </row>
+    <row r="206" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>8</v>
       </c>
@@ -6663,8 +6711,12 @@
         <v>0</v>
       </c>
       <c r="H206" s="10"/>
-      <c r="I206" s="10"/>
-      <c r="J206" s="10"/>
+      <c r="I206" s="10">
+        <v>0</v>
+      </c>
+      <c r="J206" s="10">
+        <v>0</v>
+      </c>
       <c r="M206">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6692,8 +6744,10 @@
       <c r="W206" s="19" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X206" s="10"/>
+      <c r="Y206" s="10"/>
+    </row>
+    <row r="207" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>8</v>
       </c>
@@ -6706,7 +6760,7 @@
       </c>
       <c r="D207" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E207" s="10">
         <f t="shared" si="3"/>
@@ -6720,10 +6774,10 @@
       </c>
       <c r="H207" s="10"/>
       <c r="I207" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J207" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K207" t="s">
         <v>42</v>
@@ -6737,7 +6791,7 @@
       </c>
       <c r="N207">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O207">
         <f t="shared" si="4"/>
@@ -6758,8 +6812,10 @@
       <c r="W207" s="19" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X207" s="10"/>
+      <c r="Y207" s="10"/>
+    </row>
+    <row r="208" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>8</v>
       </c>
@@ -6785,8 +6841,12 @@
         <v>0</v>
       </c>
       <c r="H208" s="10"/>
-      <c r="I208" s="10"/>
-      <c r="J208" s="10"/>
+      <c r="I208" s="10">
+        <v>0</v>
+      </c>
+      <c r="J208" s="10">
+        <v>0</v>
+      </c>
       <c r="M208">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6801,8 +6861,10 @@
       </c>
       <c r="V208" s="19"/>
       <c r="W208" s="19"/>
-    </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X208" s="10"/>
+      <c r="Y208" s="10"/>
+    </row>
+    <row r="209" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>8</v>
       </c>
@@ -6815,7 +6877,7 @@
       </c>
       <c r="D209" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E209" s="10">
         <f t="shared" si="3"/>
@@ -6829,10 +6891,10 @@
       </c>
       <c r="H209" s="10"/>
       <c r="I209" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J209" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K209" t="s">
         <v>42</v>
@@ -6846,7 +6908,7 @@
       </c>
       <c r="N209">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O209">
         <f t="shared" si="4"/>
@@ -6870,8 +6932,10 @@
       <c r="W209" s="19" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X209" s="10"/>
+      <c r="Y209" s="10"/>
+    </row>
+    <row r="210" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>8</v>
       </c>
@@ -6897,8 +6961,12 @@
         <v>0</v>
       </c>
       <c r="H210" s="10"/>
-      <c r="I210" s="10"/>
-      <c r="J210" s="10"/>
+      <c r="I210" s="10">
+        <v>0</v>
+      </c>
+      <c r="J210" s="10">
+        <v>0</v>
+      </c>
       <c r="M210">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6926,8 +6994,10 @@
       <c r="W210" s="19" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X210" s="10"/>
+      <c r="Y210" s="10"/>
+    </row>
+    <row r="211" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>8</v>
       </c>
@@ -6940,7 +7010,7 @@
       </c>
       <c r="D211" s="10">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E211" s="10">
         <f t="shared" si="3"/>
@@ -6954,10 +7024,10 @@
       </c>
       <c r="H211" s="10"/>
       <c r="I211" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J211" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K211" t="s">
         <v>42</v>
@@ -6971,7 +7041,7 @@
       </c>
       <c r="N211">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O211">
         <f t="shared" si="4"/>
@@ -6992,8 +7062,10 @@
       <c r="W211" s="19" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X211" s="10"/>
+      <c r="Y211" s="10"/>
+    </row>
+    <row r="212" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>8</v>
       </c>
@@ -7019,8 +7091,12 @@
         <v>0</v>
       </c>
       <c r="H212" s="10"/>
-      <c r="I212" s="10"/>
-      <c r="J212" s="10"/>
+      <c r="I212" s="10">
+        <v>0</v>
+      </c>
+      <c r="J212" s="10">
+        <v>0</v>
+      </c>
       <c r="M212">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7048,8 +7124,10 @@
       <c r="W212" s="19" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X212" s="10"/>
+      <c r="Y212" s="10"/>
+    </row>
+    <row r="213" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>8</v>
       </c>
@@ -7101,8 +7179,10 @@
       </c>
       <c r="S213" s="19"/>
       <c r="T213" s="19"/>
-    </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X213" s="10"/>
+      <c r="Y213" s="10"/>
+    </row>
+    <row r="214" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>8</v>
       </c>
@@ -7128,8 +7208,12 @@
         <v>0</v>
       </c>
       <c r="H214" s="10"/>
-      <c r="I214" s="10"/>
-      <c r="J214" s="10"/>
+      <c r="I214" s="10">
+        <v>0</v>
+      </c>
+      <c r="J214" s="10">
+        <v>0</v>
+      </c>
       <c r="M214">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7144,8 +7228,10 @@
       </c>
       <c r="S214" s="19"/>
       <c r="T214" s="19"/>
-    </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X214" s="10"/>
+      <c r="Y214" s="10"/>
+    </row>
+    <row r="215" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>8</v>
       </c>
@@ -7158,7 +7244,7 @@
       </c>
       <c r="D215" s="10">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E215" s="10">
         <f t="shared" si="3"/>
@@ -7172,10 +7258,10 @@
       </c>
       <c r="H215" s="10"/>
       <c r="I215" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J215" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K215" t="s">
         <v>42</v>
@@ -7189,7 +7275,7 @@
       </c>
       <c r="N215">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O215">
         <f t="shared" si="4"/>
@@ -7197,8 +7283,10 @@
       </c>
       <c r="S215" s="19"/>
       <c r="T215" s="19"/>
-    </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X215" s="10"/>
+      <c r="Y215" s="10"/>
+    </row>
+    <row r="216" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>8</v>
       </c>
@@ -7224,8 +7312,12 @@
         <v>0</v>
       </c>
       <c r="H216" s="10"/>
-      <c r="I216" s="10"/>
-      <c r="J216" s="10"/>
+      <c r="I216" s="10">
+        <v>0</v>
+      </c>
+      <c r="J216" s="10">
+        <v>0</v>
+      </c>
       <c r="M216">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7240,8 +7332,10 @@
       </c>
       <c r="S216" s="19"/>
       <c r="T216" s="19"/>
-    </row>
-    <row r="217" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X216" s="10"/>
+      <c r="Y216" s="10"/>
+    </row>
+    <row r="217" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>8</v>
       </c>
@@ -7267,8 +7361,12 @@
         <v>0</v>
       </c>
       <c r="H217" s="10"/>
-      <c r="I217" s="10"/>
-      <c r="J217" s="10"/>
+      <c r="I217" s="10">
+        <v>0</v>
+      </c>
+      <c r="J217" s="10">
+        <v>0</v>
+      </c>
       <c r="M217">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7283,8 +7381,10 @@
       </c>
       <c r="S217" s="19"/>
       <c r="T217" s="19"/>
-    </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X217" s="10"/>
+      <c r="Y217" s="10"/>
+    </row>
+    <row r="218" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>8</v>
       </c>
@@ -7310,8 +7410,12 @@
         <v>0</v>
       </c>
       <c r="H218" s="10"/>
-      <c r="I218" s="10"/>
-      <c r="J218" s="10"/>
+      <c r="I218" s="10">
+        <v>0</v>
+      </c>
+      <c r="J218" s="10">
+        <v>0</v>
+      </c>
       <c r="M218">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7324,8 +7428,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X218" s="10"/>
+      <c r="Y218" s="10"/>
+    </row>
+    <row r="219" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>8</v>
       </c>
@@ -7375,8 +7481,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X219" s="10"/>
+      <c r="Y219" s="10"/>
+    </row>
+    <row r="220" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>8</v>
       </c>
@@ -7402,8 +7510,12 @@
         <v>0</v>
       </c>
       <c r="H220" s="10"/>
-      <c r="I220" s="10"/>
-      <c r="J220" s="10"/>
+      <c r="I220" s="10">
+        <v>0</v>
+      </c>
+      <c r="J220" s="10">
+        <v>0</v>
+      </c>
       <c r="M220">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7416,8 +7528,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X220" s="10"/>
+      <c r="Y220" s="10"/>
+    </row>
+    <row r="221" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>8</v>
       </c>
@@ -7443,8 +7557,12 @@
         <v>0</v>
       </c>
       <c r="H221" s="10"/>
-      <c r="I221" s="10"/>
-      <c r="J221" s="10"/>
+      <c r="I221" s="10">
+        <v>0</v>
+      </c>
+      <c r="J221" s="10">
+        <v>0</v>
+      </c>
       <c r="M221">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7457,8 +7575,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X221" s="10"/>
+      <c r="Y221" s="10"/>
+    </row>
+    <row r="222" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>8</v>
       </c>
@@ -7484,8 +7604,12 @@
         <v>0</v>
       </c>
       <c r="H222" s="10"/>
-      <c r="I222" s="10"/>
-      <c r="J222" s="10"/>
+      <c r="I222" s="10">
+        <v>0</v>
+      </c>
+      <c r="J222" s="10">
+        <v>0</v>
+      </c>
       <c r="M222">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7498,8 +7622,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X222" s="10"/>
+      <c r="Y222" s="10"/>
+    </row>
+    <row r="223" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>8</v>
       </c>
@@ -7525,8 +7651,12 @@
         <v>0</v>
       </c>
       <c r="H223" s="10"/>
-      <c r="I223" s="10"/>
-      <c r="J223" s="10"/>
+      <c r="I223" s="10">
+        <v>0</v>
+      </c>
+      <c r="J223" s="10">
+        <v>0</v>
+      </c>
       <c r="M223">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7539,8 +7669,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X223" s="10"/>
+      <c r="Y223" s="10"/>
+    </row>
+    <row r="224" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>8</v>
       </c>
@@ -7566,8 +7698,12 @@
         <v>0</v>
       </c>
       <c r="H224" s="10"/>
-      <c r="I224" s="10"/>
-      <c r="J224" s="10"/>
+      <c r="I224" s="10">
+        <v>0</v>
+      </c>
+      <c r="J224" s="10">
+        <v>0</v>
+      </c>
       <c r="M224">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7580,8 +7716,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X224" s="10"/>
+      <c r="Y224" s="10"/>
+    </row>
+    <row r="225" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>8</v>
       </c>
@@ -7607,8 +7745,12 @@
         <v>0</v>
       </c>
       <c r="H225" s="10"/>
-      <c r="I225" s="10"/>
-      <c r="J225" s="10"/>
+      <c r="I225" s="10">
+        <v>0</v>
+      </c>
+      <c r="J225" s="10">
+        <v>0</v>
+      </c>
       <c r="M225">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7621,8 +7763,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X225" s="10"/>
+      <c r="Y225" s="10"/>
+    </row>
+    <row r="226" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>9</v>
       </c>
@@ -7647,7 +7791,12 @@
       <c r="G226">
         <v>0</v>
       </c>
-      <c r="I226" s="10"/>
+      <c r="I226" s="10">
+        <v>0</v>
+      </c>
+      <c r="J226" s="10">
+        <v>0</v>
+      </c>
       <c r="M226">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7660,8 +7809,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X226" s="10"/>
+      <c r="Y226" s="10"/>
+    </row>
+    <row r="227" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>9</v>
       </c>
@@ -7711,8 +7862,10 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X227" s="10"/>
+      <c r="Y227" s="10"/>
+    </row>
+    <row r="228" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>9</v>
       </c>
@@ -7738,8 +7891,12 @@
         <v>0</v>
       </c>
       <c r="H228" s="10"/>
-      <c r="I228" s="10"/>
-      <c r="J228" s="10"/>
+      <c r="I228" s="10">
+        <v>0</v>
+      </c>
+      <c r="J228" s="10">
+        <v>0</v>
+      </c>
       <c r="M228">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7752,8 +7909,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X228" s="10"/>
+      <c r="Y228" s="10"/>
+    </row>
+    <row r="229" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>9</v>
       </c>
@@ -7766,7 +7925,7 @@
       </c>
       <c r="D229" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E229" s="10">
         <f t="shared" si="3"/>
@@ -7780,10 +7939,10 @@
       </c>
       <c r="H229" s="10"/>
       <c r="I229" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J229" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K229" t="s">
         <v>43</v>
@@ -7797,14 +7956,16 @@
       </c>
       <c r="N229">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O229">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X229" s="10"/>
+      <c r="Y229" s="10"/>
+    </row>
+    <row r="230" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>9</v>
       </c>
@@ -7830,8 +7991,12 @@
         <v>0</v>
       </c>
       <c r="H230" s="10"/>
-      <c r="I230" s="10"/>
-      <c r="J230" s="10"/>
+      <c r="I230" s="10">
+        <v>0</v>
+      </c>
+      <c r="J230" s="10">
+        <v>0</v>
+      </c>
       <c r="M230">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7844,8 +8009,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X230" s="10"/>
+      <c r="Y230" s="10"/>
+    </row>
+    <row r="231" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>9</v>
       </c>
@@ -7895,8 +8062,10 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X231" s="10"/>
+      <c r="Y231" s="10"/>
+    </row>
+    <row r="232" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>9</v>
       </c>
@@ -7922,8 +8091,12 @@
         <v>0</v>
       </c>
       <c r="H232" s="10"/>
-      <c r="I232" s="10"/>
-      <c r="J232" s="10"/>
+      <c r="I232" s="10">
+        <v>0</v>
+      </c>
+      <c r="J232" s="10">
+        <v>0</v>
+      </c>
       <c r="M232">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7936,8 +8109,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X232" s="10"/>
+      <c r="Y232" s="10"/>
+    </row>
+    <row r="233" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>9</v>
       </c>
@@ -7950,7 +8125,7 @@
       </c>
       <c r="D233" s="10">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E233" s="10">
         <f t="shared" si="3"/>
@@ -7964,10 +8139,10 @@
       </c>
       <c r="H233" s="10"/>
       <c r="I233" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J233" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K233" t="s">
         <v>43</v>
@@ -7981,14 +8156,16 @@
       </c>
       <c r="N233">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O233">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X233" s="10"/>
+      <c r="Y233" s="10"/>
+    </row>
+    <row r="234" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>9</v>
       </c>
@@ -8013,7 +8190,12 @@
       <c r="G234">
         <v>0</v>
       </c>
-      <c r="I234" s="10"/>
+      <c r="I234" s="10">
+        <v>0</v>
+      </c>
+      <c r="J234" s="10">
+        <v>0</v>
+      </c>
       <c r="M234">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8026,8 +8208,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X234" s="10"/>
+      <c r="Y234" s="10"/>
+    </row>
+    <row r="235" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>9</v>
       </c>
@@ -8040,7 +8224,7 @@
       </c>
       <c r="D235" s="10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E235" s="10">
         <f t="shared" si="3"/>
@@ -8054,10 +8238,10 @@
       </c>
       <c r="H235" s="10"/>
       <c r="I235" s="10" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J235" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K235" t="s">
         <v>43</v>
@@ -8071,14 +8255,16 @@
       </c>
       <c r="N235">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O235">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X235" s="10"/>
+      <c r="Y235" s="10"/>
+    </row>
+    <row r="236" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>9</v>
       </c>
@@ -8104,8 +8290,12 @@
         <v>0</v>
       </c>
       <c r="H236" s="10"/>
-      <c r="I236" s="10"/>
-      <c r="J236" s="10"/>
+      <c r="I236" s="10">
+        <v>0</v>
+      </c>
+      <c r="J236" s="10">
+        <v>0</v>
+      </c>
       <c r="M236">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8118,8 +8308,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X236" s="10"/>
+      <c r="Y236" s="10"/>
+    </row>
+    <row r="237" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>9</v>
       </c>
@@ -8132,7 +8324,7 @@
       </c>
       <c r="D237" s="10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E237" s="10">
         <f t="shared" si="3"/>
@@ -8146,10 +8338,10 @@
       </c>
       <c r="H237" s="10"/>
       <c r="I237" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J237" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K237" t="s">
         <v>43</v>
@@ -8163,14 +8355,16 @@
       </c>
       <c r="N237">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O237">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X237" s="10"/>
+      <c r="Y237" s="10"/>
+    </row>
+    <row r="238" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>9</v>
       </c>
@@ -8196,8 +8390,12 @@
         <v>0</v>
       </c>
       <c r="H238" s="10"/>
-      <c r="I238" s="10"/>
-      <c r="J238" s="10"/>
+      <c r="I238" s="10">
+        <v>0</v>
+      </c>
+      <c r="J238" s="10">
+        <v>0</v>
+      </c>
       <c r="M238">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8210,8 +8408,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X238" s="10"/>
+      <c r="Y238" s="10"/>
+    </row>
+    <row r="239" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>9</v>
       </c>
@@ -8224,7 +8424,7 @@
       </c>
       <c r="D239" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E239" s="10">
         <f t="shared" si="3"/>
@@ -8238,10 +8438,10 @@
       </c>
       <c r="H239" s="10"/>
       <c r="I239" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J239" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K239" t="s">
         <v>43</v>
@@ -8255,14 +8455,16 @@
       </c>
       <c r="N239">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O239">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X239" s="10"/>
+      <c r="Y239" s="10"/>
+    </row>
+    <row r="240" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>9</v>
       </c>
@@ -8288,8 +8490,12 @@
         <v>0</v>
       </c>
       <c r="H240" s="10"/>
-      <c r="I240" s="10"/>
-      <c r="J240" s="10"/>
+      <c r="I240" s="10">
+        <v>0</v>
+      </c>
+      <c r="J240" s="10">
+        <v>0</v>
+      </c>
       <c r="M240">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8302,8 +8508,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X240" s="10"/>
+      <c r="Y240" s="10"/>
+    </row>
+    <row r="241" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>9</v>
       </c>
@@ -8316,7 +8524,7 @@
       </c>
       <c r="D241" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E241" s="10">
         <f t="shared" si="3"/>
@@ -8330,10 +8538,10 @@
       </c>
       <c r="H241" s="10"/>
       <c r="I241" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J241" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K241" t="s">
         <v>43</v>
@@ -8347,14 +8555,16 @@
       </c>
       <c r="N241">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O241">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X241" s="10"/>
+      <c r="Y241" s="10"/>
+    </row>
+    <row r="242" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>9</v>
       </c>
@@ -8379,7 +8589,12 @@
       <c r="G242">
         <v>0</v>
       </c>
-      <c r="I242" s="10"/>
+      <c r="I242" s="10">
+        <v>0</v>
+      </c>
+      <c r="J242" s="10">
+        <v>0</v>
+      </c>
       <c r="M242">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8392,8 +8607,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X242" s="10"/>
+      <c r="Y242" s="10"/>
+    </row>
+    <row r="243" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>9</v>
       </c>
@@ -8406,7 +8623,7 @@
       </c>
       <c r="D243" s="10">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E243" s="10">
         <f t="shared" si="3"/>
@@ -8420,10 +8637,10 @@
       </c>
       <c r="H243" s="10"/>
       <c r="I243" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="J243" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K243" t="s">
         <v>43</v>
@@ -8437,14 +8654,16 @@
       </c>
       <c r="N243">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O243">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X243" s="10"/>
+      <c r="Y243" s="10"/>
+    </row>
+    <row r="244" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>9</v>
       </c>
@@ -8470,8 +8689,12 @@
         <v>0</v>
       </c>
       <c r="H244" s="10"/>
-      <c r="I244" s="10"/>
-      <c r="J244" s="10"/>
+      <c r="I244" s="10">
+        <v>0</v>
+      </c>
+      <c r="J244" s="10">
+        <v>0</v>
+      </c>
       <c r="M244">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8484,8 +8707,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X244" s="10"/>
+      <c r="Y244" s="10"/>
+    </row>
+    <row r="245" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>9</v>
       </c>
@@ -8535,8 +8760,10 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X245" s="10"/>
+      <c r="Y245" s="10"/>
+    </row>
+    <row r="246" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>9</v>
       </c>
@@ -8562,8 +8789,12 @@
         <v>0</v>
       </c>
       <c r="H246" s="10"/>
-      <c r="I246" s="10"/>
-      <c r="J246" s="10"/>
+      <c r="I246" s="10">
+        <v>0</v>
+      </c>
+      <c r="J246" s="10">
+        <v>0</v>
+      </c>
       <c r="M246">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8576,8 +8807,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X246" s="10"/>
+      <c r="Y246" s="10"/>
+    </row>
+    <row r="247" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>9</v>
       </c>
@@ -8590,7 +8823,7 @@
       </c>
       <c r="D247" s="10">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E247" s="10">
         <f t="shared" si="3"/>
@@ -8604,10 +8837,10 @@
       </c>
       <c r="H247" s="10"/>
       <c r="I247" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J247" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K247" t="s">
         <v>43</v>
@@ -8621,14 +8854,16 @@
       </c>
       <c r="N247">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O247">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X247" s="10"/>
+      <c r="Y247" s="10"/>
+    </row>
+    <row r="248" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>9</v>
       </c>
@@ -8654,8 +8889,12 @@
         <v>0</v>
       </c>
       <c r="H248" s="10"/>
-      <c r="I248" s="10"/>
-      <c r="J248" s="10"/>
+      <c r="I248" s="10">
+        <v>0</v>
+      </c>
+      <c r="J248" s="10">
+        <v>0</v>
+      </c>
       <c r="M248">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8668,8 +8907,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X248" s="10"/>
+      <c r="Y248" s="10"/>
+    </row>
+    <row r="249" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>9</v>
       </c>
@@ -8695,8 +8936,12 @@
         <v>0</v>
       </c>
       <c r="H249" s="10"/>
-      <c r="I249" s="10"/>
-      <c r="J249" s="10"/>
+      <c r="I249" s="10">
+        <v>0</v>
+      </c>
+      <c r="J249" s="10">
+        <v>0</v>
+      </c>
       <c r="M249">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8709,8 +8954,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X249" s="10"/>
+      <c r="Y249" s="10"/>
+    </row>
+    <row r="250" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>9</v>
       </c>
@@ -8735,7 +8982,12 @@
       <c r="G250">
         <v>0</v>
       </c>
-      <c r="I250" s="10"/>
+      <c r="I250" s="10">
+        <v>0</v>
+      </c>
+      <c r="J250" s="10">
+        <v>0</v>
+      </c>
       <c r="M250">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8748,8 +9000,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X250" s="10"/>
+      <c r="Y250" s="10"/>
+    </row>
+    <row r="251" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>9</v>
       </c>
@@ -8799,8 +9053,10 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X251" s="10"/>
+      <c r="Y251" s="10"/>
+    </row>
+    <row r="252" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>9</v>
       </c>
@@ -8826,7 +9082,12 @@
         <v>0</v>
       </c>
       <c r="H252" s="10"/>
-      <c r="J252" s="10"/>
+      <c r="I252" s="10">
+        <v>0</v>
+      </c>
+      <c r="J252" s="10">
+        <v>0</v>
+      </c>
       <c r="M252">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8839,8 +9100,10 @@
         <f t="shared" ref="O252:O257" si="8">IF(K252=$P$192, 0, IF(K252="S", 0, 1))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X252" s="10"/>
+      <c r="Y252" s="10"/>
+    </row>
+    <row r="253" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>9</v>
       </c>
@@ -8866,7 +9129,12 @@
         <v>0</v>
       </c>
       <c r="H253" s="10"/>
-      <c r="J253" s="10"/>
+      <c r="I253" s="10">
+        <v>0</v>
+      </c>
+      <c r="J253" s="10">
+        <v>0</v>
+      </c>
       <c r="M253">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8879,8 +9147,10 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X253" s="10"/>
+      <c r="Y253" s="10"/>
+    </row>
+    <row r="254" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>9</v>
       </c>
@@ -8906,7 +9176,12 @@
         <v>0</v>
       </c>
       <c r="H254" s="10"/>
-      <c r="J254" s="10"/>
+      <c r="I254" s="10">
+        <v>0</v>
+      </c>
+      <c r="J254" s="10">
+        <v>0</v>
+      </c>
       <c r="M254">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8919,8 +9194,10 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X254" s="10"/>
+      <c r="Y254" s="10"/>
+    </row>
+    <row r="255" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>9</v>
       </c>
@@ -8946,7 +9223,12 @@
         <v>0</v>
       </c>
       <c r="H255" s="10"/>
-      <c r="J255" s="10"/>
+      <c r="I255" s="10">
+        <v>0</v>
+      </c>
+      <c r="J255" s="10">
+        <v>0</v>
+      </c>
       <c r="M255">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8959,8 +9241,10 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X255" s="10"/>
+      <c r="Y255" s="10"/>
+    </row>
+    <row r="256" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>9</v>
       </c>
@@ -8986,7 +9270,12 @@
         <v>0</v>
       </c>
       <c r="H256" s="10"/>
-      <c r="J256" s="10"/>
+      <c r="I256" s="10">
+        <v>0</v>
+      </c>
+      <c r="J256" s="10">
+        <v>0</v>
+      </c>
       <c r="M256">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -8999,8 +9288,10 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X256" s="10"/>
+      <c r="Y256" s="10"/>
+    </row>
+    <row r="257" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>9</v>
       </c>
@@ -9026,7 +9317,12 @@
         <v>0</v>
       </c>
       <c r="H257" s="10"/>
-      <c r="J257" s="10"/>
+      <c r="I257" s="10">
+        <v>0</v>
+      </c>
+      <c r="J257" s="10">
+        <v>0</v>
+      </c>
       <c r="M257">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -9039,8 +9335,10 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="X257" s="10"/>
+      <c r="Y257" s="10"/>
+    </row>
+    <row r="258" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>12</v>
       </c>
@@ -9063,7 +9361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>12</v>
       </c>
@@ -9086,7 +9384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>12</v>
       </c>
@@ -9109,7 +9407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>12</v>
       </c>
@@ -9132,7 +9430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>12</v>
       </c>
@@ -9155,7 +9453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>12</v>
       </c>
@@ -9178,7 +9476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>12</v>
       </c>
@@ -9201,7 +9499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>12</v>
       </c>
@@ -9224,7 +9522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>12</v>
       </c>
@@ -9247,7 +9545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>12</v>
       </c>
@@ -9270,7 +9568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>12</v>
       </c>
@@ -9293,7 +9591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>12</v>
       </c>
@@ -9316,7 +9614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>12</v>
       </c>
@@ -9339,7 +9637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>12</v>
       </c>
@@ -9362,7 +9660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>12</v>
       </c>
@@ -9785,8 +10083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F259E-EF3B-4E40-949C-0C8D5E45A455}">
   <dimension ref="A1:G289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16448,7 +16746,7 @@
   <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="B40:D40"/>
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18479,7 +18777,7 @@
   <dimension ref="B4:T211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:J18"/>
+      <selection activeCell="E29" sqref="C29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22114,10 +22412,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC2B2D4-17CC-374D-879B-0E44BE06E68A}">
-  <dimension ref="B3:AB85"/>
+  <dimension ref="B3:AB115"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:D85"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="P52" sqref="P52:P115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22790,7 +23088,7 @@
       </c>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>8</v>
       </c>
@@ -22801,7 +23099,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>8</v>
       </c>
@@ -22810,7 +23108,7 @@
       </c>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>8</v>
       </c>
@@ -22821,7 +23119,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>8</v>
       </c>
@@ -22830,7 +23128,7 @@
       </c>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>8</v>
       </c>
@@ -22841,7 +23139,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>8</v>
       </c>
@@ -22850,7 +23148,7 @@
       </c>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>8</v>
       </c>
@@ -22860,8 +23158,32 @@
       <c r="D39" s="10" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P39" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="R39" s="10">
+        <v>0</v>
+      </c>
+      <c r="S39" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="T39" s="10">
+        <v>0</v>
+      </c>
+      <c r="U39" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="V39" s="10">
+        <v>0</v>
+      </c>
+      <c r="W39" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>8</v>
       </c>
@@ -22869,8 +23191,32 @@
         <v>19</v>
       </c>
       <c r="D40" s="10"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P40" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="R40" s="10">
+        <v>0</v>
+      </c>
+      <c r="S40" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="T40" s="10">
+        <v>0</v>
+      </c>
+      <c r="U40" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="V40" s="10">
+        <v>0</v>
+      </c>
+      <c r="W40" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>8</v>
       </c>
@@ -22880,8 +23226,32 @@
       <c r="D41" s="10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P41" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="R41" s="10">
+        <v>0</v>
+      </c>
+      <c r="S41" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="T41" s="10">
+        <v>0</v>
+      </c>
+      <c r="U41" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="V41" s="10">
+        <v>0</v>
+      </c>
+      <c r="W41" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>8</v>
       </c>
@@ -22889,8 +23259,32 @@
         <v>21</v>
       </c>
       <c r="D42" s="10"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P42" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="R42" s="10">
+        <v>0</v>
+      </c>
+      <c r="S42" s="10">
+        <v>0</v>
+      </c>
+      <c r="T42" s="10">
+        <v>0</v>
+      </c>
+      <c r="U42" s="10">
+        <v>0</v>
+      </c>
+      <c r="V42" s="10">
+        <v>0</v>
+      </c>
+      <c r="W42" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>8</v>
       </c>
@@ -22900,8 +23294,16 @@
       <c r="D43" s="10" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
+      <c r="W43" s="10"/>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>8</v>
       </c>
@@ -22909,8 +23311,32 @@
         <v>23</v>
       </c>
       <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P44" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="R44" s="10">
+        <v>0</v>
+      </c>
+      <c r="S44" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="T44" s="10">
+        <v>0</v>
+      </c>
+      <c r="U44" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="V44" s="10">
+        <v>0</v>
+      </c>
+      <c r="W44" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>8</v>
       </c>
@@ -22918,8 +23344,32 @@
         <v>24</v>
       </c>
       <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P45" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="R45" s="10">
+        <v>0</v>
+      </c>
+      <c r="S45" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="T45" s="10">
+        <v>0</v>
+      </c>
+      <c r="U45" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="V45" s="10">
+        <v>0</v>
+      </c>
+      <c r="W45" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>8</v>
       </c>
@@ -22927,8 +23377,32 @@
         <v>25</v>
       </c>
       <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P46" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="R46" s="10">
+        <v>0</v>
+      </c>
+      <c r="S46" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="T46" s="10">
+        <v>0</v>
+      </c>
+      <c r="U46" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="V46" s="10">
+        <v>0</v>
+      </c>
+      <c r="W46" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>8</v>
       </c>
@@ -22938,8 +23412,32 @@
       <c r="D47" s="10" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P47" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="R47" s="10">
+        <v>0</v>
+      </c>
+      <c r="S47" s="10">
+        <v>0</v>
+      </c>
+      <c r="T47" s="10">
+        <v>0</v>
+      </c>
+      <c r="U47" s="10">
+        <v>0</v>
+      </c>
+      <c r="V47" s="10">
+        <v>0</v>
+      </c>
+      <c r="W47" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>8</v>
       </c>
@@ -22947,8 +23445,9 @@
         <v>27</v>
       </c>
       <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="W48" s="10"/>
+    </row>
+    <row r="49" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>8</v>
       </c>
@@ -22957,7 +23456,7 @@
       </c>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>8</v>
       </c>
@@ -22966,7 +23465,7 @@
       </c>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>8</v>
       </c>
@@ -22975,7 +23474,7 @@
       </c>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B52">
         <v>8</v>
       </c>
@@ -22983,8 +23482,33 @@
         <v>31</v>
       </c>
       <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P52" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="10">
+        <v>0</v>
+      </c>
+      <c r="R52" s="10">
+        <v>0</v>
+      </c>
+      <c r="S52" s="10">
+        <v>0</v>
+      </c>
+      <c r="T52" s="10"/>
+      <c r="U52" s="10">
+        <v>0</v>
+      </c>
+      <c r="V52" s="10">
+        <v>0</v>
+      </c>
+      <c r="W52" s="10">
+        <v>0</v>
+      </c>
+      <c r="X52" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B53">
         <v>8</v>
       </c>
@@ -22992,16 +23516,66 @@
         <v>32</v>
       </c>
       <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P53" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q53" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="R53" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="S53" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="T53" s="10"/>
+      <c r="U53" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="V53" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="W53" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="X53" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>9</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P54" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="10">
+        <v>0</v>
+      </c>
+      <c r="R54" s="10">
+        <v>0</v>
+      </c>
+      <c r="S54" s="10">
+        <v>0</v>
+      </c>
+      <c r="T54" s="10"/>
+      <c r="U54" s="10">
+        <v>0</v>
+      </c>
+      <c r="V54" s="10">
+        <v>0</v>
+      </c>
+      <c r="W54" s="10">
+        <v>0</v>
+      </c>
+      <c r="X54" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>9</v>
       </c>
@@ -23011,8 +23585,33 @@
       <c r="D55" s="10" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P55" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q55" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="R55" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="S55" s="10">
+        <v>0</v>
+      </c>
+      <c r="T55" s="10"/>
+      <c r="U55" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="V55" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="W55" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="X55" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>9</v>
       </c>
@@ -23020,8 +23619,33 @@
         <v>3</v>
       </c>
       <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P56" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="10">
+        <v>0</v>
+      </c>
+      <c r="R56" s="10">
+        <v>0</v>
+      </c>
+      <c r="S56" s="10">
+        <v>0</v>
+      </c>
+      <c r="T56" s="10"/>
+      <c r="U56" s="10">
+        <v>0</v>
+      </c>
+      <c r="V56" s="10">
+        <v>0</v>
+      </c>
+      <c r="W56" s="10">
+        <v>0</v>
+      </c>
+      <c r="X56" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B57">
         <v>9</v>
       </c>
@@ -23031,8 +23655,33 @@
       <c r="D57" s="10" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P57" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q57" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="R57" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="S57" s="10">
+        <v>0</v>
+      </c>
+      <c r="T57" s="10"/>
+      <c r="U57" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="V57" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="W57" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="X57" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>9</v>
       </c>
@@ -23040,8 +23689,33 @@
         <v>5</v>
       </c>
       <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P58" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="10">
+        <v>0</v>
+      </c>
+      <c r="R58" s="10">
+        <v>0</v>
+      </c>
+      <c r="S58" s="10">
+        <v>0</v>
+      </c>
+      <c r="T58" s="10"/>
+      <c r="U58" s="10">
+        <v>0</v>
+      </c>
+      <c r="V58" s="10">
+        <v>0</v>
+      </c>
+      <c r="W58" s="10">
+        <v>0</v>
+      </c>
+      <c r="X58" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B59">
         <v>9</v>
       </c>
@@ -23051,8 +23725,34 @@
       <c r="D59" s="10" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P59" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q59" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="R59" s="10">
+        <v>0</v>
+      </c>
+      <c r="S59" s="10">
+        <v>0</v>
+      </c>
+      <c r="T59" s="10"/>
+      <c r="U59" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="V59" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="W59" s="10">
+        <v>0</v>
+      </c>
+      <c r="X59" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="10"/>
+    </row>
+    <row r="60" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>9</v>
       </c>
@@ -23060,8 +23760,11 @@
         <v>7</v>
       </c>
       <c r="D60" s="10"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P60" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B61">
         <v>9</v>
       </c>
@@ -23071,16 +23774,22 @@
       <c r="D61" s="10" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P61" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B62">
         <v>9</v>
       </c>
       <c r="C62">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P62" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B63">
         <v>9</v>
       </c>
@@ -23090,8 +23799,11 @@
       <c r="D63" s="10" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P63" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B64">
         <v>9</v>
       </c>
@@ -23099,8 +23811,11 @@
         <v>11</v>
       </c>
       <c r="D64" s="10"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P64" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B65">
         <v>9</v>
       </c>
@@ -23110,8 +23825,11 @@
       <c r="D65" s="10" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P65" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B66">
         <v>9</v>
       </c>
@@ -23119,8 +23837,11 @@
         <v>13</v>
       </c>
       <c r="D66" s="10"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P66" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B67">
         <v>9</v>
       </c>
@@ -23130,8 +23851,11 @@
       <c r="D67" s="10" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P67" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B68">
         <v>9</v>
       </c>
@@ -23139,8 +23863,11 @@
         <v>15</v>
       </c>
       <c r="D68" s="10"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P68" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B69">
         <v>9</v>
       </c>
@@ -23150,16 +23877,22 @@
       <c r="D69" s="10" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P69" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B70">
         <v>9</v>
       </c>
       <c r="C70">
         <v>17</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P70" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>9</v>
       </c>
@@ -23169,8 +23902,11 @@
       <c r="D71" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P71" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>9</v>
       </c>
@@ -23178,8 +23914,11 @@
         <v>19</v>
       </c>
       <c r="D72" s="10"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P72" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B73">
         <v>9</v>
       </c>
@@ -23189,8 +23928,11 @@
       <c r="D73" s="10" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P73" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B74">
         <v>9</v>
       </c>
@@ -23198,8 +23940,11 @@
         <v>21</v>
       </c>
       <c r="D74" s="10"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P74" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B75">
         <v>9</v>
       </c>
@@ -23209,8 +23954,11 @@
       <c r="D75" s="10" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P75" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B76">
         <v>9</v>
       </c>
@@ -23218,8 +23966,11 @@
         <v>23</v>
       </c>
       <c r="D76" s="10"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P76" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B77">
         <v>9</v>
       </c>
@@ -23227,16 +23978,22 @@
         <v>24</v>
       </c>
       <c r="D77" s="10"/>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P77" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B78">
         <v>9</v>
       </c>
       <c r="C78">
         <v>25</v>
       </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P78" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B79">
         <v>9</v>
       </c>
@@ -23246,8 +24003,11 @@
       <c r="D79" s="10" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P79" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B80">
         <v>9</v>
       </c>
@@ -23255,8 +24015,11 @@
         <v>27</v>
       </c>
       <c r="D80" s="10"/>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P80" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B81">
         <v>9</v>
       </c>
@@ -23264,8 +24027,11 @@
         <v>28</v>
       </c>
       <c r="D81" s="10"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P81" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B82">
         <v>9</v>
       </c>
@@ -23273,8 +24039,11 @@
         <v>29</v>
       </c>
       <c r="D82" s="10"/>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P82" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>9</v>
       </c>
@@ -23282,8 +24051,11 @@
         <v>30</v>
       </c>
       <c r="D83" s="10"/>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P83" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B84">
         <v>9</v>
       </c>
@@ -23291,8 +24063,11 @@
         <v>31</v>
       </c>
       <c r="D84" s="10"/>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="P84" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B85">
         <v>9</v>
       </c>
@@ -23300,6 +24075,159 @@
         <v>32</v>
       </c>
       <c r="D85" s="10"/>
+      <c r="P85" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P86" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P87" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P88" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P89" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P90" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P91" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P92" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P93" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P94" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P95" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P96" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P97" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P98" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P99" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="100" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P100" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P101" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P102" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P103" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P104" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P105" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="106" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P106" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P107" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P108" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P109" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="110" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P110" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P111" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P112" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P113" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P114" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P115" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update for MCPPMT DQM
</commit_message>
<xml_diff>
--- a/mapping/mapping_TB2021July_v1.xlsx
+++ b/mapping/mapping_TB2021July_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khwang/scratch/TB2023July/preparation/dev_230622/TB2023/mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F06F2A6-4263-D642-8759-C0E922A95027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE262DF-0C00-6B40-B183-0C382B51F29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23080" yWindow="500" windowWidth="45720" windowHeight="28300" activeTab="1" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
+    <workbookView xWindow="23080" yWindow="500" windowWidth="45720" windowHeight="28300" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
   </bookViews>
   <sheets>
     <sheet name="dynamic" sheetId="1" r:id="rId1"/>
@@ -1007,9 +1007,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FA2B49-E75F-9B4E-BCDE-F5B7F2A15CFB}">
   <dimension ref="A1:Y289"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W233" sqref="W233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10083,8 +10083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F259E-EF3B-4E40-949C-0C8D5E45A455}">
   <dimension ref="A1:G289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="B247" sqref="B247:B248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding aux detector : External Trigger
</commit_message>
<xml_diff>
--- a/mapping/mapping_TB2021July_v1.xlsx
+++ b/mapping/mapping_TB2021July_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khwang/scratch/TB2023July/preparation/dev_230622/TB2023/mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khwang/scratch/TB2023July/preparation/dev_230628/TB2023/mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE262DF-0C00-6B40-B183-0C382B51F29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1850379D-B36C-E24F-A1AA-407D14B06FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23080" yWindow="500" windowWidth="45720" windowHeight="28300" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
   </bookViews>
   <sheets>
     <sheet name="dynamic" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="MCP&amp;SIPM" sheetId="4" r:id="rId3"/>
     <sheet name="case" sheetId="2" r:id="rId4"/>
     <sheet name="generic" sheetId="5" r:id="rId5"/>
+    <sheet name="Aux" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="173">
   <si>
     <t>MID</t>
   </si>
@@ -542,12 +543,30 @@
   <si>
     <t>mid</t>
   </si>
+  <si>
+    <t>Aux</t>
+  </si>
+  <si>
+    <t>ext</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>nCannel</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -568,6 +587,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -670,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -691,6 +717,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,9 +1034,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FA2B49-E75F-9B4E-BCDE-F5B7F2A15CFB}">
   <dimension ref="A1:Y289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W233" sqref="W233"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9369,10 +9396,10 @@
         <v>2</v>
       </c>
       <c r="C259">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D259">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E259">
         <v>0</v>
@@ -9553,10 +9580,10 @@
         <v>10</v>
       </c>
       <c r="C267">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D267">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E267">
         <v>0</v>
@@ -10083,8 +10110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F259E-EF3B-4E40-949C-0C8D5E45A455}">
   <dimension ref="A1:G289"/>
   <sheetViews>
-    <sheetView topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="B247" sqref="B247:B248"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16031,10 +16058,10 @@
         <v>2</v>
       </c>
       <c r="C259">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D259">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E259">
         <v>0</v>
@@ -16215,10 +16242,10 @@
         <v>10</v>
       </c>
       <c r="C267">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D267">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E267">
         <v>0</v>
@@ -22414,8 +22441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC2B2D4-17CC-374D-879B-0E44BE06E68A}">
   <dimension ref="B3:AB115"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="P52" sqref="P52:P115"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24232,4 +24259,115 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF455B5-8885-4C4E-A014-FA339AED39A6}">
+  <dimension ref="D12:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D12" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D13" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="20">
+        <v>12</v>
+      </c>
+      <c r="G13" s="20">
+        <v>2</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20">
+        <v>4</v>
+      </c>
+      <c r="J13" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D14" s="20"/>
+      <c r="E14" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" s="20">
+        <v>12</v>
+      </c>
+      <c r="G14" s="20">
+        <v>10</v>
+      </c>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20">
+        <v>4</v>
+      </c>
+      <c r="J14" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="20">
+        <v>6</v>
+      </c>
+      <c r="J17" s="20">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update mapping - adding Coincidence, Cerenkov counter
</commit_message>
<xml_diff>
--- a/mapping/mapping_TB2021July_v1.xlsx
+++ b/mapping/mapping_TB2021July_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khwang/scratch/TB2023July/preparation/dev_230628/TB2023/mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khwang/scratch/TB2023July/preparation/dev_230703/TB2023/mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1850379D-B36C-E24F-A1AA-407D14B06FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15052BB-E1F0-2A4B-BF2F-AF22FED13C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
   </bookViews>
@@ -1035,8 +1035,8 @@
   <dimension ref="A1:Y289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1048576"/>
+      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E278" sqref="E278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9534,10 +9534,10 @@
         <v>8</v>
       </c>
       <c r="C265">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D265">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E265">
         <v>0</v>
@@ -9718,10 +9718,10 @@
         <v>16</v>
       </c>
       <c r="C273">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D273">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E273">
         <v>0</v>
@@ -9948,10 +9948,10 @@
         <v>26</v>
       </c>
       <c r="C283">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D283">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E283">
         <v>0</v>
@@ -10110,8 +10110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F259E-EF3B-4E40-949C-0C8D5E45A455}">
   <dimension ref="A1:G289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="R297" sqref="R297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16196,10 +16196,10 @@
         <v>8</v>
       </c>
       <c r="C265">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D265">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E265">
         <v>0</v>
@@ -16380,10 +16380,10 @@
         <v>16</v>
       </c>
       <c r="C273">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D273">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E273">
         <v>0</v>
@@ -16610,10 +16610,10 @@
         <v>26</v>
       </c>
       <c r="C283">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D283">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E283">
         <v>0</v>

</xml_diff>

<commit_message>
update mapping : adding extra fiber trigger
</commit_message>
<xml_diff>
--- a/mapping/mapping_TB2021July_v1.xlsx
+++ b/mapping/mapping_TB2021July_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khwang/Library/Caches/com.binarynights.ForkLift-3/FileCache/5ED5FD0B-F080-4877-B269-FCA1365913D7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C85F0F8-672A-774F-8E65-81C3527FBB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EF0C76-0253-BD43-A83A-DF88CAD01B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="5" xr2:uid="{9904E546-8807-0449-B43D-5949530D5B54}"/>
   </bookViews>
   <sheets>
     <sheet name="dynamic" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="178">
   <si>
     <t>MID</t>
   </si>
@@ -561,6 +561,21 @@
   <si>
     <t>Case</t>
   </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>T1N</t>
+  </si>
+  <si>
+    <t>T2N</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T3N</t>
+  </si>
 </sst>
 </file>
 
@@ -9918,7 +9933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F259E-EF3B-4E40-949C-0C8D5E45A455}">
   <dimension ref="A1:G289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
@@ -18611,7 +18626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6155975-9163-6745-86DE-64EA3CD700DC}">
   <dimension ref="B4:T211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E29" sqref="C29:E29"/>
     </sheetView>
   </sheetViews>
@@ -24071,10 +24086,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF455B5-8885-4C4E-A014-FA339AED39A6}">
-  <dimension ref="D12:J17"/>
+  <dimension ref="D12:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24106,10 +24121,10 @@
         <v>169</v>
       </c>
       <c r="F13" s="20">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G13" s="20">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20">
@@ -24125,10 +24140,10 @@
         <v>170</v>
       </c>
       <c r="F14" s="20">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G14" s="20">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20">
@@ -24138,40 +24153,125 @@
         <v>2</v>
       </c>
     </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+    </row>
     <row r="16" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
+      <c r="E16" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="I16" s="20">
+        <v>4</v>
+      </c>
+      <c r="J16" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="E17" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="I17" s="20">
+        <v>4</v>
+      </c>
+      <c r="J17" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="E18" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>19</v>
+      </c>
+      <c r="I18" s="20">
+        <v>4</v>
+      </c>
+      <c r="J18" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="E19" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="I19" s="20">
+        <v>4</v>
+      </c>
+      <c r="J19" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
         <v>116</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>12</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="I16">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="I21">
         <v>6</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
         <v>12</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="I17" s="20">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="I22" s="20">
         <v>6</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J22" s="20">
         <v>2</v>
       </c>
     </row>

</xml_diff>